<commit_message>
feat: register user and asistence
</commit_message>
<xml_diff>
--- a/frontend/src/assets/templates/Template_users.xlsx
+++ b/frontend/src/assets/templates/Template_users.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\welin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77EB8E69-19DF-41DC-A6ED-A2BD9BD45F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166AFFCC-CABD-4EED-A1C5-7F34DE654C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{BFFB81AB-BF91-4E51-919D-1BEDE4B65AA6}"/>
+    <workbookView xWindow="12255" yWindow="4845" windowWidth="10365" windowHeight="4830" xr2:uid="{BFFB81AB-BF91-4E51-919D-1BEDE4B65AA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla de asignaturas" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>name</t>
   </si>
@@ -51,13 +49,16 @@
   </si>
   <si>
     <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>identityDocument</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -437,21 +438,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE7AE046-D6E0-482A-B8FF-4AE23F8AB6B7}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.875" customWidth="1"/>
+    <col min="2" max="2" width="17.875" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,8 +468,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="D8" s="1"/>
     </row>
   </sheetData>

</xml_diff>